<commit_message>
space-type: add acronym column in template
</commit_message>
<xml_diff>
--- a/templates/spacetype_template.xlsx
+++ b/templates/spacetype_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\Siba\Siba_be\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\siba-be\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F7C42F-ACBE-48BE-A040-CDFD5F6FA04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A96978-BDAF-4210-B142-69892EE298F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4845" yWindow="4455" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>name</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Medium description</t>
+  </si>
+  <si>
+    <t>acronym</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -384,51 +393,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>